<commit_message>
header footer content idea
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B3" t="n">
+        <v>22</v>
+      </c>
+      <c r="C3" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3" t="n">
+        <v>22</v>
+      </c>
+      <c r="E3" t="n">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>